<commit_message>
Fix parse numeric sku bug
</commit_message>
<xml_diff>
--- a/spec/support/products.xlsx
+++ b/spec/support/products.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="15" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="5" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>sku</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>property3</t>
-  </si>
-  <si>
-    <t>1234a</t>
   </si>
   <si>
     <t>Product 1</t>
@@ -74,7 +71,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -94,11 +91,6 @@
     <font>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -144,9 +136,8 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
@@ -168,11 +159,11 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6"/>
+      <selection activeCell="B7" activeCellId="0" pane="topLeft" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -196,43 +187,43 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>6000</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -258,7 +249,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -283,7 +274,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>